<commit_message>
Add bug report for Rozetka website
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302E0211-DB0A-4F9F-9201-D0EC0C1EE904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2F0B77-DA15-4C80-A86F-F59F581948FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -55,13 +55,120 @@
   </si>
   <si>
     <t>Attachments</t>
+  </si>
+  <si>
+    <t>BR1</t>
+  </si>
+  <si>
+    <t>BR2</t>
+  </si>
+  <si>
+    <t>BR3</t>
+  </si>
+  <si>
+    <t>BR4</t>
+  </si>
+  <si>
+    <t>BR5</t>
+  </si>
+  <si>
+    <t>BR6</t>
+  </si>
+  <si>
+    <t>BR7</t>
+  </si>
+  <si>
+    <t>BR8</t>
+  </si>
+  <si>
+    <t>BR9</t>
+  </si>
+  <si>
+    <t>BR10</t>
+  </si>
+  <si>
+    <t>BR11</t>
+  </si>
+  <si>
+    <t>BR12</t>
+  </si>
+  <si>
+    <t>BR13</t>
+  </si>
+  <si>
+    <t>BR14</t>
+  </si>
+  <si>
+    <t>BR15</t>
+  </si>
+  <si>
+    <t>BR16</t>
+  </si>
+  <si>
+    <t>BR17</t>
+  </si>
+  <si>
+    <t>BR18</t>
+  </si>
+  <si>
+    <t>BR19</t>
+  </si>
+  <si>
+    <t>BR20</t>
+  </si>
+  <si>
+    <t>BR21</t>
+  </si>
+  <si>
+    <t>BR22</t>
+  </si>
+  <si>
+    <t>BR23</t>
+  </si>
+  <si>
+    <t>BR24</t>
+  </si>
+  <si>
+    <t>BR25</t>
+  </si>
+  <si>
+    <t>•Go to https://rozetka.com.ua</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Filter apllied</t>
+  </si>
+  <si>
+    <t>Price filter does not apply in catagories: "Ноутбуки", "Комп'ютери, неттопи, моноблоки", "Монітори", "Мобільні телефони", "Телевізори" when input value is less than default value</t>
+  </si>
+  <si>
+    <t>1.Go to category "Смартфони, ТВ і електроніка" -"Мобільні телефони"
+2.Input value "1" in field of minimal price value
+3.Click "OK" button or press Enter
+Note: In some other category the default value is 1 and price filter works properly</t>
+  </si>
+  <si>
+    <t>•Windows 10 Pro x64 bit (v. 21H2)
+•Opera (v.89.0.4447.83)
+•Google Chrome (v.104.0.5112.79)</t>
+  </si>
+  <si>
+    <t>1. Price filter does not apply</t>
+  </si>
+  <si>
+    <t>2. Price filter applied</t>
+  </si>
+  <si>
+    <t>Filter does not apply. Fields of minimum and maximum price marked in red. "OK" button does not work.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +179,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -125,11 +238,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -137,6 +289,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,18 +594,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -464,307 +643,381 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="A16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="A17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="A19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="A20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="A23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="A24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="A25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="A26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add links for attachments to BR1
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2F0B77-DA15-4C80-A86F-F59F581948FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4839299-AA9E-4657-AFC5-B881AE4A42DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +185,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,8 +286,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -299,13 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -314,8 +317,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -597,7 +607,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,12 +681,12 @@
       <c r="I2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
@@ -685,7 +695,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="11" t="s">
         <v>42</v>
       </c>
     </row>
@@ -693,14 +703,14 @@
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="10"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1018,7 +1028,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{13F608D6-7943-46F7-9C71-368A0F11DE84}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{166EC488-2B33-46E4-9BC8-242261FAFE44}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add BR2 and organise attachment folder
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3CC899-C513-405F-89EF-F6F5E4846172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47F2066-7D7A-423C-9700-F83EAFAF4173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -155,13 +155,27 @@
 •Google Chrome (v.104.0.5112.79)</t>
   </si>
   <si>
-    <t>1. Price filter does not apply</t>
-  </si>
-  <si>
-    <t>2. Price filter applied</t>
-  </si>
-  <si>
     <t>Filter does not apply. Fields of minimum and maximum price marked in red. "OK" button does not work.</t>
+  </si>
+  <si>
+    <t>•Go to https://dominos.ua/uk/kyiv/</t>
+  </si>
+  <si>
+    <t>1.Change language to English by clicking dropdown button at the top of website
+2.Click on "Sign in" button
+3.Click "Sign in button"(without filling any fields) to invoke the error message</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>The same bug appears on each page with error messages(e.g. Registration, Checkout, Forgot password?  etc. pages)</t>
+  </si>
+  <si>
+    <t>The language of error messages  do not change after switching to English</t>
+  </si>
+  <si>
+    <t>The language of error messages  change after switching to English</t>
   </si>
 </sst>
 </file>
@@ -212,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -260,33 +274,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -301,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -310,7 +300,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -325,21 +315,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,24 +600,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="36.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
     <col min="6" max="6" width="71.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" customWidth="1"/>
     <col min="8" max="8" width="27.140625" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" customWidth="1"/>
+    <col min="10" max="11" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,8 +648,11 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -693,46 +675,65 @@
         <v>37</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="10" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7"/>
+      <c r="F3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -743,10 +744,11 @@
       <c r="H5" s="6"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -757,10 +759,11 @@
       <c r="H6" s="6"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -771,10 +774,11 @@
       <c r="H7" s="6"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -785,10 +789,11 @@
       <c r="H8" s="6"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -799,10 +804,11 @@
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -813,10 +819,11 @@
       <c r="H10" s="6"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -827,10 +834,11 @@
       <c r="H11" s="6"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -841,10 +849,11 @@
       <c r="H12" s="6"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -855,10 +864,11 @@
       <c r="H13" s="6"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -869,10 +879,11 @@
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -883,10 +894,11 @@
       <c r="H15" s="6"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -897,10 +909,11 @@
       <c r="H16" s="6"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -911,10 +924,11 @@
       <c r="H17" s="6"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -925,10 +939,11 @@
       <c r="H18" s="6"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -939,10 +954,11 @@
       <c r="H19" s="6"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -953,10 +969,11 @@
       <c r="H20" s="6"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -967,10 +984,11 @@
       <c r="H21" s="6"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -981,10 +999,11 @@
       <c r="H22" s="6"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -995,10 +1014,11 @@
       <c r="H23" s="6"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1009,10 +1029,11 @@
       <c r="H24" s="6"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1023,33 +1044,16 @@
       <c r="H25" s="6"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{13F608D6-7943-46F7-9C71-368A0F11DE84}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{166EC488-2B33-46E4-9BC8-242261FAFE44}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add link to BR3 attachment
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47D7B87-366D-47AE-B5AF-36CE096F3CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573A368A-206E-4A21-849D-9A1DD050F373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -627,7 +627,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +775,9 @@
       <c r="I4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1103,8 +1105,9 @@
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{58D8CC7C-F0D5-4DEF-909C-4F01FC6C8ED8}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{B2961E52-6918-45A4-A270-08B6877E847E}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{3C33F18B-2FC9-4366-BDA1-D1D0A7294E1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add link to BR4 attachement
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EEBC40-4583-407E-9DC2-D23C43087CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2786223-0D64-44BE-9726-A68E584AC475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -70,66 +70,6 @@
   </si>
   <si>
     <t>BR5</t>
-  </si>
-  <si>
-    <t>BR6</t>
-  </si>
-  <si>
-    <t>BR7</t>
-  </si>
-  <si>
-    <t>BR8</t>
-  </si>
-  <si>
-    <t>BR9</t>
-  </si>
-  <si>
-    <t>BR10</t>
-  </si>
-  <si>
-    <t>BR11</t>
-  </si>
-  <si>
-    <t>BR12</t>
-  </si>
-  <si>
-    <t>BR13</t>
-  </si>
-  <si>
-    <t>BR14</t>
-  </si>
-  <si>
-    <t>BR15</t>
-  </si>
-  <si>
-    <t>BR16</t>
-  </si>
-  <si>
-    <t>BR17</t>
-  </si>
-  <si>
-    <t>BR18</t>
-  </si>
-  <si>
-    <t>BR19</t>
-  </si>
-  <si>
-    <t>BR20</t>
-  </si>
-  <si>
-    <t>BR21</t>
-  </si>
-  <si>
-    <t>BR22</t>
-  </si>
-  <si>
-    <t>BR23</t>
-  </si>
-  <si>
-    <t>BR24</t>
-  </si>
-  <si>
-    <t>BR25</t>
   </si>
   <si>
     <t>•Go to https://rozetka.com.ua</t>
@@ -333,12 +273,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -642,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,451 +627,163 @@
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>47</v>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>42</v>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="5"/>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1140,8 +791,9 @@
     <hyperlink ref="J2" r:id="rId1" xr:uid="{58D8CC7C-F0D5-4DEF-909C-4F01FC6C8ED8}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{B2961E52-6918-45A4-A270-08B6877E847E}"/>
     <hyperlink ref="J4" r:id="rId3" xr:uid="{3C33F18B-2FC9-4366-BDA1-D1D0A7294E1A}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{240998FD-C84E-4C3D-9785-3089066F126F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add BR5 for robby shop
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2786223-0D64-44BE-9726-A68E584AC475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8435F160-D1CF-41AC-89FD-5F418CF3B840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -158,6 +158,37 @@
   </si>
   <si>
     <t>Total amount includes item price only, until checkout page is opened</t>
+  </si>
+  <si>
+    <t>•Go to https://robby.com.ua</t>
+  </si>
+  <si>
+    <t>1.Change language to Ukrainian by clicking dropdown button at the top of website
+2.Click on " Клієнт-центр" dropdown button and "Реєстрація" link
+3.Click on "Продовжити" button(without filling email and password field)</t>
+  </si>
+  <si>
+    <t>Red error message "Некоректна адреса електронної пошти!" is displayed under email field
+Red error message "Пароль має бути від 4 до 20 символів!" is displayed under password field</t>
+  </si>
+  <si>
+    <t>Red error message "regexp error" is displayed under email field
+Red error message "byLength error" is displayed under password field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no validation on email </t>
+  </si>
+  <si>
+    <t>Registration page localization in Ukrainian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error messages for Email and password fileds displayed incorrectly on Registration page after changing language to Ukrainian </t>
+  </si>
+  <si>
+    <t>BR6</t>
+  </si>
+  <si>
+    <t>BR7</t>
   </si>
 </sst>
 </file>
@@ -273,7 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,6 +330,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -581,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +627,7 @@
     <col min="4" max="4" width="36.85546875" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" customWidth="1"/>
     <col min="6" max="6" width="71.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
     <col min="8" max="8" width="27.140625" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.5703125" customWidth="1"/>
@@ -770,20 +805,70 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Add link to attachemnt for BR5
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8435F160-D1CF-41AC-89FD-5F418CF3B840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B7B976-8177-4804-9F81-D6C5E54E2890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -176,9 +176,6 @@
 Red error message "byLength error" is displayed under password field</t>
   </si>
   <si>
-    <t xml:space="preserve">no validation on email </t>
-  </si>
-  <si>
     <t>Registration page localization in Ukrainian</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>BR7</t>
+  </si>
+  <si>
+    <t>no validation on email on registration</t>
   </si>
 </sst>
 </file>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +816,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>41</v>
@@ -833,17 +833,19 @@
       <c r="I6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -855,12 +857,12 @@
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -877,8 +879,9 @@
     <hyperlink ref="J3" r:id="rId2" xr:uid="{B2961E52-6918-45A4-A270-08B6877E847E}"/>
     <hyperlink ref="J4" r:id="rId3" xr:uid="{3C33F18B-2FC9-4366-BDA1-D1D0A7294E1A}"/>
     <hyperlink ref="J5" r:id="rId4" xr:uid="{240998FD-C84E-4C3D-9785-3089066F126F}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{C35BDF61-05BC-4DD0-B8DD-3A468CE5618C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 3 BR for Registration page on Robby shop
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B7B976-8177-4804-9F81-D6C5E54E2890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D22E70-8134-4F6F-92C6-CE026ED0ECE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -142,16 +142,10 @@
     <t>"Checkout" button become "Замовити" button</t>
   </si>
   <si>
-    <t>Minor</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
     <t>1.Select item/items on total amount below 250 UAH and click "To cart" button</t>
-  </si>
-  <si>
-    <t>Delivery cost for total amount below 250 UAH is not displayed on homepage until checkout page is opened</t>
   </si>
   <si>
     <t>Total amount along with delivery cost calculated</t>
@@ -176,9 +170,6 @@
 Red error message "byLength error" is displayed under password field</t>
   </si>
   <si>
-    <t>Registration page localization in Ukrainian</t>
-  </si>
-  <si>
     <t xml:space="preserve">Error messages for Email and password fileds displayed incorrectly on Registration page after changing language to Ukrainian </t>
   </si>
   <si>
@@ -188,7 +179,60 @@
     <t>BR7</t>
   </si>
   <si>
-    <t>no validation on email on registration</t>
+    <t>1.Click on " Клієнт-центр" dropdown button and "Реєстрація" link</t>
+  </si>
+  <si>
+    <t>User is not registered, "email" field is marked in red and message "Введіть коректну адресу електронної пошти." is displayed</t>
+  </si>
+  <si>
+    <t>User is registred and redirected to Profile page and receive message: "ОБЛІКОВА ЗАПИС УСПІШНО СТВОРЕНА!"</t>
+  </si>
+  <si>
+    <t>1.Click on " Клієнт-центр" dropdown button and "Реєстрація" link
+2. Fill out "email" field with invalid data-тест3@gmail.com
+3.Fill out "Пароль"and "Підтвердіть пароль" field with valid data-1234
+4.Fill out "Iм'я" field with valid data-Іван
+5.Fill out "Прізвище" field with valid data-Карпенко
+6.Fill out "Телефон" field with valid data-+380999999999
+7.Click on "Продовжити" button</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>•Go to https://robby.com.ua
+•Change language to Ukrainian by clicking dropdown button at the top of website</t>
+  </si>
+  <si>
+    <t>Page is translated to Ukrainian</t>
+  </si>
+  <si>
+    <t>Word "Main" and "password" has not been translated</t>
+  </si>
+  <si>
+    <t>BR8</t>
+  </si>
+  <si>
+    <t>Hover state of  text on"Продовжити" button does not meet contrast behavior on Registration page</t>
+  </si>
+  <si>
+    <t>Incorrect Ukrainian localization on Registration page</t>
+  </si>
+  <si>
+    <t>No validation in E-mail field on Registration page when user input cyrillic symbols</t>
+  </si>
+  <si>
+    <t>Delivery cost for total amount below 250 UAH is not displayed on Homepage until checkout page is opened</t>
+  </si>
+  <si>
+    <t>Hover states  of text meets contrast</t>
+  </si>
+  <si>
+    <t>Text merges with background</t>
+  </si>
+  <si>
+    <t>1.Click on " Клієнт-центр" dropdown button and "Реєстрація" link
+2.Hover over "Продовжити" button</t>
   </si>
 </sst>
 </file>
@@ -304,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,13 +371,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -616,10 +665,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +747,7 @@
       <c r="I2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="12" t="s">
         <v>25</v>
       </c>
       <c r="K2" s="5" t="s">
@@ -732,7 +782,7 @@
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -767,7 +817,7 @@
       <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="4"/>
@@ -777,30 +827,30 @@
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="H5" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="4"/>
@@ -810,67 +860,126 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="H7" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Add links for BR
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D22E70-8134-4F6F-92C6-CE026ED0ECE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E78CEF1-CA99-4252-807B-3A948A553E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -669,7 +669,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +916,9 @@
       <c r="I7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -947,7 +949,9 @@
       <c r="I8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -978,7 +982,9 @@
       <c r="I9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="K9" s="4"/>
     </row>
   </sheetData>
@@ -989,8 +995,11 @@
     <hyperlink ref="J4" r:id="rId3" xr:uid="{3C33F18B-2FC9-4366-BDA1-D1D0A7294E1A}"/>
     <hyperlink ref="J5" r:id="rId4" xr:uid="{240998FD-C84E-4C3D-9785-3089066F126F}"/>
     <hyperlink ref="J6" r:id="rId5" xr:uid="{C35BDF61-05BC-4DD0-B8DD-3A468CE5618C}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{8C6CB81B-6F0B-433C-B38A-1280C8BF84E5}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{8EF0434B-EDD5-4A58-9BF2-364F9E561D99}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{A3620470-669E-4C46-BA76-7A8FD46D3957}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update link to attachements
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED8A919-85FB-4D82-A39A-BC28FA78A596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97233931-D3CC-4B46-8448-7D740D1E7CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,9 +672,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add new bug reports for Dota 2 game
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4931614-57C1-4856-A3BB-103B101F9D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F78C864-82CC-48F4-9018-BF77C6A77406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>BR5</t>
-  </si>
-  <si>
-    <t>•Go to https://rozetka.com.ua</t>
   </si>
   <si>
     <t>Low</t>
@@ -83,23 +80,13 @@
 •Google Chrome (v.104.0.5112.79)</t>
   </si>
   <si>
-    <t>•Go to https://dominos.ua/uk/kyiv/</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
     <t>Link to attachments</t>
   </si>
   <si>
-    <t xml:space="preserve">•Go to https://dominos.ua/uk/kyiv/
-•Change language to English </t>
-  </si>
-  <si>
     <t>Medium</t>
-  </si>
-  <si>
-    <t>•Go to https://robby.com.ua</t>
   </si>
   <si>
     <t>Red error message "Некоректна адреса електронної пошти!" is displayed under email field
@@ -130,10 +117,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>•Go to https://robby.com.ua
-•Change language to Ukrainian by clicking dropdown button at the top of website</t>
-  </si>
-  <si>
     <t>Page is translated to Ukrainian</t>
   </si>
   <si>
@@ -207,11 +190,6 @@
     <t xml:space="preserve">Error messages for Email and password fileds are displayed incorrectly on Registration page after changing language to Ukrainian </t>
   </si>
   <si>
-    <t>1.Change language to Ukrainian by clicking dropdown button at the top of website
-2.Click the " Клієнт-центр" dropdown button and "Реєстрація" link
-3.Click the "Продовжити" button(without filling email and password field)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Error messages for Email and password fileds are displayed incorrectly on Registration page after changing language to Ukrainian.  ("regexp error" for email field and "byLength error" for password field)
 </t>
   </si>
@@ -238,6 +216,118 @@
   </si>
   <si>
     <t>Hover state of  text on the "Продовжити" button is not meet contrast behavior on the Registration page. Text merges with background</t>
+  </si>
+  <si>
+    <t>BR9</t>
+  </si>
+  <si>
+    <t>BR10</t>
+  </si>
+  <si>
+    <t>BR11</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Win. Battlefield. The free "Town Portal Scroll" item is shown in the stash after buying and selling "Boots of travel" item</t>
+  </si>
+  <si>
+    <t>1. Go out of base stash range and buy "Town Portal Scroll" item
+2. Go to base and buy "Boots of travel" item
+3. Sell "Boots of travel" item
+4. Pay attention to the "Town Portal Scroll" item quantity in the stash</t>
+  </si>
+  <si>
+    <t>The quantity of "Town Portal Scroll" item is decreased in the stash after buying and selling "Boots of travel" item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The free "Town Portal Scroll" item is shown in the stash after buying and selling "Boots of travel" item
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•Windows 10 Pro x64 bit (v. 21H2)
+</t>
+  </si>
+  <si>
+    <t>Win. Battle field. Arc Warden hero The teleport animation is displayed on the battlefield after using "Tempest double" during copies' teleport</t>
+  </si>
+  <si>
+    <t>1. Launch the game
+2. Go to Demo mode with Arc Warden hero
+3. Use "-lvlup 30" cheat code and learn "Tempest double" skill
+4. Buy "Boots of travel" item</t>
+  </si>
+  <si>
+    <t>1.Go to https://rozetka.com.ua</t>
+  </si>
+  <si>
+    <t>1.Go to https://dominos.ua/uk/kyiv/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Go to https://dominos.ua/uk/kyiv/
+2.Change language to English </t>
+  </si>
+  <si>
+    <t>1.Go to https://robby.com.ua</t>
+  </si>
+  <si>
+    <t>1.Go to https://robby.com.ua
+2.Change language to Ukrainian by clicking dropdown button at the top of website</t>
+  </si>
+  <si>
+    <t>1.Launch the game
+2.Create lobby with cheat mode, pick any hero and start the game
+3.Use "-gold 99999" cheat code</t>
+  </si>
+  <si>
+    <t>1.Use "Tempest double" skill and use "Boots of travel" item by copy
+2.Use "Tempest double" skill during teleport animation by original hero
+3. Pay attention to the teleport animation</t>
+  </si>
+  <si>
+    <t>1.Change language to Ukrainian by clicking dropdown button at the top of website
+2.Click the " Клієнт-центр" dropdown button and "Реєстрація" link
+3.Click the "Продовжити" button(without filling email and password field)
+4. Pay attention to the error message language</t>
+  </si>
+  <si>
+    <t>The teleport animation is not displayed on the battlefield after using "Tempest double" during copies' teleport</t>
+  </si>
+  <si>
+    <t>The teleport animation is displayed on the battlefield after using "Tempest double" during copies' teleport</t>
+  </si>
+  <si>
+    <t>Win. Battlefield. Dark Seer hero. The "Normal Punch" skill effect is shown after buying and selling "Aghanim's scepter"</t>
+  </si>
+  <si>
+    <t>•The game: Dota 2 Patch #7.32b
+•To reproduce this bug the "Town Portal Scroll" item should be in the stash
+•This item could be used and sold</t>
+  </si>
+  <si>
+    <t>•The game: Dota 2 Patch #7.32b
+•The teleport animation is displayed every time Arc Warden using "Tempest double" during copies' teleport</t>
+  </si>
+  <si>
+    <t>1. Launch the game
+2. Go to Demo mode with Dark Seer hero
+3. Create enemy hero by clicking "+Enemy" button or using “-createhero templar enemy" cheat code</t>
+  </si>
+  <si>
+    <t>1.Buy "Aghanim's scepter" item by Dark Seer
+2. Sell "Aghanim's scepter" item by Dark Seer and right click on Templar Assassin hero
+3. Pay attention to the "Aghanim's scepter" Dark Seer punch animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The "Normal Punch" skill effect is not shown after buying and selling "Aghanim's scepter"</t>
+  </si>
+  <si>
+    <t>The "Normal Punch" skill effect is shown after buying and selling "Aghanim's scepter"</t>
+  </si>
+  <si>
+    <t>•The game: Dota 2 Patch #7.32b
+•The "Normal Punch" skill effect is shown only with the first punch to enemy hero or creep</t>
   </si>
 </sst>
 </file>
@@ -344,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -359,9 +449,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -379,20 +466,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -424,7 +519,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -438,49 +533,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -767,367 +820,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
     <col min="6" max="6" width="71.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" style="16" customWidth="1"/>
     <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.5703125" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>19</v>
+      <c r="K1" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>20</v>
+      <c r="J2" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>35</v>
+      <c r="B5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="150" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>35</v>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="J9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="1"/>
+      <c r="D12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B9">
+  <conditionalFormatting sqref="B2:B12">
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B9">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Medium">
+  <conditionalFormatting sqref="B2:B12">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",B2)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C12">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Trivial">
+      <formula>NOT(ISERROR(SEARCH("Trivial",C2)))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C9">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Blocker">
-      <formula>NOT(ISERROR(SEARCH("Blocker",C2)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Minor">
+      <formula>NOT(ISERROR(SEARCH("Minor",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Critical">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Major">
+      <formula>NOT(ISERROR(SEARCH("Major",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Critical">
       <formula>NOT(ISERROR(SEARCH("Critical",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Major">
-      <formula>NOT(ISERROR(SEARCH("Major",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Minor">
-      <formula>NOT(ISERROR(SEARCH("Minor",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Trivial">
-      <formula>NOT(ISERROR(SEARCH("Trivial",C2)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Blocker">
+      <formula>NOT(ISERROR(SEARCH("Blocker",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9" xr:uid="{11138892-488B-490E-A5A2-FA68C68E2733}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B12" xr:uid="{11138892-488B-490E-A5A2-FA68C68E2733}">
       <formula1>"High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{66F1B395-12AF-4852-8471-D4CB028F0FD4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C12" xr:uid="{66F1B395-12AF-4852-8471-D4CB028F0FD4}">
       <formula1>"Blocker, Critical, Major, Minor, Trivial"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add links for BR9-BR11 attachements
</commit_message>
<xml_diff>
--- a/Bug reports/Bug reports.xlsx
+++ b/Bug reports/Bug reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Git\Projects\Test-documentation\Bug reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F78C864-82CC-48F4-9018-BF77C6A77406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F386BB-BB51-40F0-A133-D2EA870433F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -823,8 +823,8 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1172,9 @@
       <c r="I10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="6"/>
+      <c r="J10" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="K10" s="6" t="s">
         <v>78</v>
       </c>
@@ -1205,7 +1207,9 @@
       <c r="I11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="K11" s="6" t="s">
         <v>79</v>
       </c>
@@ -1238,7 +1242,9 @@
       <c r="I12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="J12" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="K12" s="2" t="s">
         <v>84</v>
       </c>
@@ -1292,8 +1298,12 @@
     <hyperlink ref="J7" r:id="rId6" xr:uid="{8C6CB81B-6F0B-433C-B38A-1280C8BF84E5}"/>
     <hyperlink ref="J8" r:id="rId7" xr:uid="{8EF0434B-EDD5-4A58-9BF2-364F9E561D99}"/>
     <hyperlink ref="J9" r:id="rId8" xr:uid="{A3620470-669E-4C46-BA76-7A8FD46D3957}"/>
+    <hyperlink ref="J10:J12" r:id="rId9" display="Link to attachments" xr:uid="{AF8BE0B2-C1C0-4E01-A0FA-C56E906B4132}"/>
+    <hyperlink ref="J10" r:id="rId10" xr:uid="{150158F3-AFBC-49B3-ADAA-F28F1BE40311}"/>
+    <hyperlink ref="J11" r:id="rId11" xr:uid="{E91CDC0F-6155-4604-B64A-A61074CDBB20}"/>
+    <hyperlink ref="J12" r:id="rId12" xr:uid="{9CF5AD1D-5AC7-4717-B18D-E190DDF68731}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>